<commit_message>
range elevation and coordinate system working, azimuth not
</commit_message>
<xml_diff>
--- a/CCP Laser feasibility study.xlsx
+++ b/CCP Laser feasibility study.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nuitenbr/Desktop/lunarspark/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5114DFC1-A70B-F148-A17E-ADACFA02E044}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF434788-CCD5-0D46-9FE1-FDFD521DE530}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="300" yWindow="2760" windowWidth="34720" windowHeight="18880" xr2:uid="{0D0644B8-F9A6-4A61-A91E-2BD3522A7E9F}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="69">
   <si>
     <t>baseline</t>
   </si>
@@ -232,6 +232,18 @@
   </si>
   <si>
     <t>inNight</t>
+  </si>
+  <si>
+    <t>power available should afford desired # of lasers</t>
+  </si>
+  <si>
+    <t>drives power available for lasers</t>
+  </si>
+  <si>
+    <t>usable energy after receiving losses</t>
+  </si>
+  <si>
+    <t>energy delivered to the surface</t>
   </si>
 </sst>
 </file>
@@ -294,7 +306,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -308,6 +320,10 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -624,8 +640,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96B0B46A-223E-4370-BADF-6F68045EC825}">
   <dimension ref="B1:W39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C3" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="T27" sqref="T27"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -656,14 +672,16 @@
         <v>6.2068965517241379</v>
       </c>
       <c r="F2" s="5">
-        <f>6.2*1.47</f>
-        <v>9.1140000000000008</v>
+        <v>6.21</v>
       </c>
       <c r="G2" s="5">
-        <v>12.5</v>
+        <v>12.42</v>
       </c>
       <c r="H2" s="5">
-        <v>25</v>
+        <v>24.84</v>
+      </c>
+      <c r="I2" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="2:23" x14ac:dyDescent="0.2">
@@ -726,15 +744,15 @@
       </c>
       <c r="F5" s="2">
         <f>F2*F3*F4/1000</f>
-        <v>3.7540565999999997</v>
+        <v>2.5578989999999999</v>
       </c>
       <c r="G5" s="2">
         <f>G2*G3*G4/1000</f>
-        <v>5.1487499999999997</v>
+        <v>5.1157979999999998</v>
       </c>
       <c r="H5" s="2">
         <f>H2*H3*H4/1000</f>
-        <v>10.297499999999999</v>
+        <v>10.231596</v>
       </c>
     </row>
     <row r="7" spans="2:23" x14ac:dyDescent="0.2">
@@ -876,15 +894,15 @@
       </c>
       <c r="F12" s="2">
         <f>F5*F11/60</f>
-        <v>6.8524046471999993</v>
+        <v>4.6690183080000001</v>
       </c>
       <c r="G12" s="2">
         <f>G5*G11/60</f>
-        <v>9.3981849999999998</v>
+        <v>9.3380366160000001</v>
       </c>
       <c r="H12" s="2">
         <f>H5*H11/60</f>
-        <v>18.79637</v>
+        <v>18.676073232</v>
       </c>
       <c r="M12" t="s">
         <v>60</v>
@@ -1166,15 +1184,15 @@
       </c>
       <c r="F17" s="1">
         <f>F12*F15*F16</f>
-        <v>0.30835820912399997</v>
+        <v>0.21010582385999999</v>
       </c>
       <c r="G17" s="1">
         <f>G12*G15*G16</f>
-        <v>0.42291832499999993</v>
+        <v>0.42021164771999997</v>
       </c>
       <c r="H17" s="1">
         <f>H12*H15*H16</f>
-        <v>0.84583664999999986</v>
+        <v>0.84042329543999994</v>
       </c>
       <c r="L17">
         <v>-60</v>
@@ -1236,15 +1254,15 @@
       </c>
       <c r="F18" s="2">
         <f>F12*F15</f>
-        <v>2.0557213941599999</v>
+        <v>1.4007054924</v>
       </c>
       <c r="G18" s="2">
         <f>G12*G15</f>
-        <v>2.8194554999999997</v>
+        <v>2.8014109847999999</v>
       </c>
       <c r="H18" s="2">
         <f>H12*H15</f>
-        <v>5.6389109999999993</v>
+        <v>5.6028219695999999</v>
       </c>
       <c r="L18">
         <v>-30</v>
@@ -1366,18 +1384,22 @@
         <f>E18/21*60*E19</f>
         <v>1.0000039211822658</v>
       </c>
-      <c r="F20" s="1">
+      <c r="F20" s="11">
         <f>F18/21*60*F19</f>
-        <v>1.4683724243999998</v>
-      </c>
-      <c r="G20" s="1">
+        <v>1.0005039231428572</v>
+      </c>
+      <c r="G20" s="11">
         <f>G18/21*60*G19</f>
-        <v>2.0138967857142855</v>
-      </c>
-      <c r="H20" s="1">
+        <v>2.0010078462857144</v>
+      </c>
+      <c r="H20" s="11">
         <f>H18/21*60*H19</f>
-        <v>4.0277935714285711</v>
-      </c>
+        <v>4.0020156925714288</v>
+      </c>
+      <c r="I20" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="J20" s="12"/>
       <c r="L20">
         <v>30</v>
       </c>
@@ -1422,6 +1444,8 @@
       </c>
     </row>
     <row r="21" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="I21" s="12"/>
+      <c r="J21" s="12"/>
       <c r="L21">
         <v>60</v>
       </c>
@@ -1477,18 +1501,20 @@
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="10">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="10">
         <f>FLOOR(G20,1)</f>
         <v>2</v>
       </c>
-      <c r="H22">
+      <c r="H22" s="10">
         <f>FLOOR(H20,1)</f>
         <v>4</v>
       </c>
+      <c r="I22" s="12"/>
+      <c r="J22" s="12"/>
       <c r="L22">
         <v>90</v>
       </c>
@@ -1717,15 +1743,18 @@
       </c>
       <c r="F26" s="1">
         <f>F20*F8/60</f>
-        <v>0.51393034853999997</v>
+        <v>0.35017637309999999</v>
       </c>
       <c r="G26" s="1">
         <f>G20*G8/60</f>
-        <v>0.70486387499999992</v>
+        <v>0.70035274619999999</v>
       </c>
       <c r="H26" s="1">
         <f>H20*H8/60</f>
-        <v>1.4097277499999998</v>
+        <v>1.4007054924</v>
+      </c>
+      <c r="I26" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="27" spans="2:23" x14ac:dyDescent="0.2">
@@ -1745,15 +1774,15 @@
       </c>
       <c r="F27" s="1">
         <f t="shared" si="8"/>
-        <v>6.4241293567499996E-2</v>
+        <v>4.3772046637499999E-2</v>
       </c>
       <c r="G27" s="1">
         <f>G26/G23</f>
-        <v>8.810798437499999E-2</v>
+        <v>8.7544093274999998E-2</v>
       </c>
       <c r="H27" s="1">
         <f>H26/H23</f>
-        <v>0.17621596874999998</v>
+        <v>0.17508818655</v>
       </c>
     </row>
     <row r="29" spans="2:23" x14ac:dyDescent="0.2">
@@ -1773,15 +1802,15 @@
       </c>
       <c r="F29" s="1">
         <f>F26*F13</f>
-        <v>5.0004033911999999</v>
+        <v>3.4071214680000002</v>
       </c>
       <c r="G29" s="1">
         <f>G26*G13</f>
-        <v>6.858134999999999</v>
+        <v>6.8142429360000003</v>
       </c>
       <c r="H29" s="1">
         <f>H26*H13</f>
-        <v>13.716269999999998</v>
+        <v>13.628485872000001</v>
       </c>
     </row>
     <row r="30" spans="2:23" x14ac:dyDescent="0.2">
@@ -1801,15 +1830,15 @@
       </c>
       <c r="F30" s="1">
         <f t="shared" si="9"/>
-        <v>0.62505042389999999</v>
+        <v>0.42589018350000002</v>
       </c>
       <c r="G30" s="1">
         <f>G29/G23</f>
-        <v>0.85726687499999987</v>
+        <v>0.85178036700000004</v>
       </c>
       <c r="H30" s="1">
         <f>H29/H23</f>
-        <v>1.7145337499999997</v>
+        <v>1.7035607340000001</v>
       </c>
     </row>
     <row r="32" spans="2:23" x14ac:dyDescent="0.2">
@@ -1832,7 +1861,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>33</v>
       </c>
@@ -1852,7 +1881,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
         <v>28</v>
       </c>
@@ -1869,18 +1898,21 @@
       </c>
       <c r="F35" s="1">
         <f t="shared" si="10"/>
-        <v>0.1747363185036</v>
+        <v>0.119059966854</v>
       </c>
       <c r="G35" s="1">
         <f>G26*G$33*G$32</f>
-        <v>0.23965371749999997</v>
+        <v>0.238119933708</v>
       </c>
       <c r="H35" s="1">
         <f>H26*H$33*H$32</f>
-        <v>0.47930743499999995</v>
-      </c>
-    </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.2">
+        <v>0.476239867416</v>
+      </c>
+      <c r="I35" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
         <v>29</v>
       </c>
@@ -1897,18 +1929,18 @@
       </c>
       <c r="F36" s="1">
         <f t="shared" si="11"/>
-        <v>2.184203981295E-2</v>
+        <v>1.488249585675E-2</v>
       </c>
       <c r="G36" s="1">
         <f>G27*G$33*G$32</f>
-        <v>2.9956714687499997E-2</v>
+        <v>2.97649917135E-2</v>
       </c>
       <c r="H36" s="1">
         <f>H27*H$33*H$32</f>
-        <v>5.9913429374999994E-2</v>
-      </c>
-    </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.2">
+        <v>5.9529983426999999E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
@@ -1916,7 +1948,7 @@
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
     </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
         <v>30</v>
       </c>
@@ -1933,18 +1965,18 @@
       </c>
       <c r="F38" s="1">
         <f t="shared" si="12"/>
-        <v>1.7001371530080001</v>
+        <v>1.1584212991200002</v>
       </c>
       <c r="G38" s="1">
         <f>G29*G$33*G$32</f>
-        <v>2.3317658999999997</v>
+        <v>2.3168425982400005</v>
       </c>
       <c r="H38" s="1">
         <f>H29*H$33*H$32</f>
-        <v>4.6635317999999994</v>
-      </c>
-    </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.2">
+        <v>4.633685196480001</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
         <v>31</v>
       </c>
@@ -1961,18 +1993,21 @@
       </c>
       <c r="F39" s="1">
         <f t="shared" si="13"/>
-        <v>0.21251714412600001</v>
+        <v>0.14480266239000003</v>
       </c>
       <c r="G39" s="1">
         <f>G30*G$33*G$32</f>
-        <v>0.29147073749999997</v>
+        <v>0.28960532478000006</v>
       </c>
       <c r="H39" s="1">
         <f>H30*H$33*H$32</f>
-        <v>0.58294147499999993</v>
+        <v>0.57921064956000012</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="I20:J22"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
updated documentation and TODO items
</commit_message>
<xml_diff>
--- a/CCP Laser feasibility study.xlsx
+++ b/CCP Laser feasibility study.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nuitenbr/Desktop/lunarspark/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF434788-CCD5-0D46-9FE1-FDFD521DE530}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD807EFE-F0A7-CE4A-8E9D-B07C9EB70685}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="300" yWindow="2760" windowWidth="34720" windowHeight="18880" xr2:uid="{0D0644B8-F9A6-4A61-A91E-2BD3522A7E9F}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="71">
   <si>
     <t>baseline</t>
   </si>
@@ -244,6 +244,12 @@
   </si>
   <si>
     <t>energy delivered to the surface</t>
+  </si>
+  <si>
+    <t>anomaly</t>
+  </si>
+  <si>
+    <t>lat</t>
   </si>
 </sst>
 </file>
@@ -641,7 +647,7 @@
   <dimension ref="B1:W39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+      <selection activeCell="V6" sqref="V6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -656,6 +662,12 @@
       <c r="H1" s="6" t="s">
         <v>0</v>
       </c>
+      <c r="N1" t="s">
+        <v>69</v>
+      </c>
+      <c r="O1" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="2" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
@@ -683,6 +695,28 @@
       <c r="I2" t="s">
         <v>66</v>
       </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>90</v>
+      </c>
+      <c r="P2">
+        <f>N2-180</f>
+        <v>-180</v>
+      </c>
+      <c r="Q2">
+        <f>MOD(P2,90)</f>
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <f>IF(N2&gt;180,-MOD(N2,180),N2)</f>
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <f>90-N2</f>
+        <v>90</v>
+      </c>
     </row>
     <row r="3" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
@@ -706,6 +740,28 @@
       <c r="H3" s="5">
         <v>1373</v>
       </c>
+      <c r="N3">
+        <v>45</v>
+      </c>
+      <c r="O3">
+        <v>45</v>
+      </c>
+      <c r="P3">
+        <f t="shared" ref="P3:P9" si="0">N3-180</f>
+        <v>-135</v>
+      </c>
+      <c r="Q3">
+        <f t="shared" ref="Q3:Q9" si="1">MOD(P3,90)</f>
+        <v>45</v>
+      </c>
+      <c r="R3">
+        <f t="shared" ref="R3:R9" si="2">IF(N3&gt;180,-MOD(N3,180),N3)</f>
+        <v>45</v>
+      </c>
+      <c r="T3">
+        <f t="shared" ref="T3:T6" si="3">90-N3</f>
+        <v>45</v>
+      </c>
     </row>
     <row r="4" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
@@ -726,6 +782,28 @@
       <c r="H4" s="4">
         <v>0.3</v>
       </c>
+      <c r="N4">
+        <v>90</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <f t="shared" si="0"/>
+        <v>-90</v>
+      </c>
+      <c r="Q4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <f t="shared" si="2"/>
+        <v>90</v>
+      </c>
+      <c r="T4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
@@ -754,6 +832,52 @@
         <f>H2*H3*H4/1000</f>
         <v>10.231596</v>
       </c>
+      <c r="N5">
+        <v>120</v>
+      </c>
+      <c r="O5">
+        <v>-30</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="0"/>
+        <v>-60</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="R5">
+        <f t="shared" si="2"/>
+        <v>120</v>
+      </c>
+      <c r="T5">
+        <f t="shared" si="3"/>
+        <v>-30</v>
+      </c>
+    </row>
+    <row r="6" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="N6">
+        <v>180</v>
+      </c>
+      <c r="O6">
+        <v>-90</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <f t="shared" si="2"/>
+        <v>180</v>
+      </c>
+      <c r="T6">
+        <f t="shared" si="3"/>
+        <v>-90</v>
+      </c>
     </row>
     <row r="7" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
@@ -777,6 +901,28 @@
       <c r="H7" s="5">
         <v>148</v>
       </c>
+      <c r="N7">
+        <v>220</v>
+      </c>
+      <c r="O7">
+        <v>-50</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="R7">
+        <f t="shared" si="2"/>
+        <v>-40</v>
+      </c>
+      <c r="T7">
+        <f>-90+MOD(N7,180)</f>
+        <v>-50</v>
+      </c>
     </row>
     <row r="8" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
@@ -800,6 +946,28 @@
       <c r="H8" s="5">
         <v>21</v>
       </c>
+      <c r="N8">
+        <v>270</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="0"/>
+        <v>90</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R8">
+        <f t="shared" si="2"/>
+        <v>-90</v>
+      </c>
+      <c r="T8">
+        <f t="shared" ref="T8:T9" si="4">-90+MOD(N8,180)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
@@ -828,6 +996,28 @@
         <f>H7-H8</f>
         <v>127</v>
       </c>
+      <c r="N9">
+        <v>330</v>
+      </c>
+      <c r="O9">
+        <v>60</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+      <c r="R9">
+        <f t="shared" si="2"/>
+        <v>-150</v>
+      </c>
+      <c r="T9">
+        <f t="shared" si="4"/>
+        <v>60</v>
+      </c>
     </row>
     <row r="10" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
@@ -971,11 +1161,11 @@
         <v>0</v>
       </c>
       <c r="Q13">
-        <f>MOD(P13+90, 360)</f>
+        <f t="shared" ref="Q13:Q25" si="5">MOD(P13+90, 360)</f>
         <v>90</v>
       </c>
       <c r="R13">
-        <f>MOD(P13+270, 360)</f>
+        <f t="shared" ref="R13:R25" si="6">MOD(P13+270, 360)</f>
         <v>270</v>
       </c>
       <c r="S13">
@@ -1004,42 +1194,42 @@
         <v>-150</v>
       </c>
       <c r="M14">
-        <f t="shared" ref="M14:M25" si="0">MOD(L14+360,360)</f>
+        <f t="shared" ref="M14:M25" si="7">MOD(L14+360,360)</f>
         <v>210</v>
       </c>
       <c r="N14">
-        <f t="shared" ref="N14:N25" si="1">L14+360</f>
+        <f t="shared" ref="N14:N25" si="8">L14+360</f>
         <v>210</v>
       </c>
       <c r="P14">
         <v>30</v>
       </c>
       <c r="Q14">
-        <f>MOD(P14+90, 360)</f>
+        <f t="shared" si="5"/>
         <v>120</v>
       </c>
       <c r="R14">
-        <f>MOD(P14+270, 360)</f>
+        <f t="shared" si="6"/>
         <v>300</v>
       </c>
       <c r="S14">
-        <f t="shared" ref="S14:S25" si="2">P14+360-90</f>
+        <f t="shared" ref="S14:S25" si="9">P14+360-90</f>
         <v>300</v>
       </c>
       <c r="T14">
-        <f t="shared" ref="T14:T25" si="3">P14+360+90</f>
+        <f t="shared" ref="T14:T25" si="10">P14+360+90</f>
         <v>480</v>
       </c>
       <c r="U14">
-        <f t="shared" ref="U14:U25" si="4">IF(M$13&lt;R14,1,0)</f>
+        <f t="shared" ref="U14:U25" si="11">IF(M$13&lt;R14,1,0)</f>
         <v>1</v>
       </c>
       <c r="V14">
-        <f t="shared" ref="V14:V25" si="5">IF($M14&lt;Q14, 1, 0)</f>
+        <f t="shared" ref="V14:V25" si="12">IF($M14&lt;Q14, 1, 0)</f>
         <v>0</v>
       </c>
       <c r="W14" t="b">
-        <f t="shared" ref="W14:W25" si="6">AND(U14:V14)</f>
+        <f t="shared" ref="W14:W25" si="13">AND(U14:V14)</f>
         <v>0</v>
       </c>
     </row>
@@ -1066,42 +1256,42 @@
         <v>-120</v>
       </c>
       <c r="M15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="7"/>
         <v>240</v>
       </c>
       <c r="N15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>240</v>
       </c>
       <c r="P15">
         <v>60</v>
       </c>
       <c r="Q15">
-        <f>MOD(P15+90, 360)</f>
+        <f t="shared" si="5"/>
         <v>150</v>
       </c>
       <c r="R15">
-        <f>MOD(P15+270, 360)</f>
+        <f t="shared" si="6"/>
         <v>330</v>
       </c>
       <c r="S15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>330</v>
       </c>
       <c r="T15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>510</v>
       </c>
       <c r="U15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="V15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="W15" t="b">
-        <f t="shared" si="6"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
     </row>
@@ -1128,42 +1318,42 @@
         <v>-90</v>
       </c>
       <c r="M16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="7"/>
         <v>270</v>
       </c>
       <c r="N16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>270</v>
       </c>
       <c r="P16" s="10">
         <v>90</v>
       </c>
       <c r="Q16" s="10">
-        <f>MOD(P16+90, 360)</f>
+        <f t="shared" si="5"/>
         <v>180</v>
       </c>
       <c r="R16" s="10">
-        <f>MOD(P16+270, 360)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="S16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>360</v>
       </c>
       <c r="T16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>540</v>
       </c>
       <c r="U16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="V16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="W16" t="b">
-        <f t="shared" si="6"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
     </row>
@@ -1198,42 +1388,42 @@
         <v>-60</v>
       </c>
       <c r="M17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="7"/>
         <v>300</v>
       </c>
       <c r="N17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>300</v>
       </c>
       <c r="P17" s="10">
         <v>120</v>
       </c>
       <c r="Q17" s="10">
-        <f>MOD(P17+90, 360)</f>
+        <f t="shared" si="5"/>
         <v>210</v>
       </c>
       <c r="R17" s="10">
-        <f>MOD(P17+270, 360)</f>
+        <f t="shared" si="6"/>
         <v>30</v>
       </c>
       <c r="S17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>390</v>
       </c>
       <c r="T17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>570</v>
       </c>
       <c r="U17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="V17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="W17" t="b">
-        <f t="shared" si="6"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
     </row>
@@ -1268,42 +1458,42 @@
         <v>-30</v>
       </c>
       <c r="M18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="7"/>
         <v>330</v>
       </c>
       <c r="N18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>330</v>
       </c>
       <c r="P18" s="10">
         <v>150</v>
       </c>
       <c r="Q18" s="10">
-        <f>MOD(P18+90, 360)</f>
+        <f t="shared" si="5"/>
         <v>240</v>
       </c>
       <c r="R18" s="10">
-        <f>MOD(P18+270, 360)</f>
+        <f t="shared" si="6"/>
         <v>60</v>
       </c>
       <c r="S18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>420</v>
       </c>
       <c r="T18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>600</v>
       </c>
       <c r="U18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="V18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="W18" t="b">
-        <f t="shared" si="6"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
     </row>
@@ -1330,42 +1520,42 @@
         <v>0</v>
       </c>
       <c r="M19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>360</v>
       </c>
       <c r="P19" s="10">
         <v>180</v>
       </c>
       <c r="Q19" s="10">
-        <f>MOD(P19+90, 360)</f>
+        <f t="shared" si="5"/>
         <v>270</v>
       </c>
       <c r="R19" s="10">
-        <f>MOD(P19+270, 360)</f>
+        <f t="shared" si="6"/>
         <v>90</v>
       </c>
       <c r="S19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>450</v>
       </c>
       <c r="T19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>630</v>
       </c>
       <c r="U19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="V19">
-        <f t="shared" si="5"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="W19" t="b">
-        <f t="shared" si="6"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
     </row>
@@ -1404,42 +1594,42 @@
         <v>30</v>
       </c>
       <c r="M20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="7"/>
         <v>30</v>
       </c>
       <c r="N20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>390</v>
       </c>
       <c r="P20" s="10">
         <v>210</v>
       </c>
       <c r="Q20" s="10">
-        <f>MOD(P20+90, 360)</f>
+        <f t="shared" si="5"/>
         <v>300</v>
       </c>
       <c r="R20" s="10">
-        <f>MOD(P20+270, 360)</f>
+        <f t="shared" si="6"/>
         <v>120</v>
       </c>
       <c r="S20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>480</v>
       </c>
       <c r="T20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>660</v>
       </c>
       <c r="U20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="V20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="W20" t="b">
-        <f t="shared" si="6"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
     </row>
@@ -1450,42 +1640,42 @@
         <v>60</v>
       </c>
       <c r="M21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="7"/>
         <v>60</v>
       </c>
       <c r="N21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>420</v>
       </c>
       <c r="P21" s="10">
         <v>240</v>
       </c>
       <c r="Q21" s="10">
-        <f>MOD(P21+90, 360)</f>
+        <f t="shared" si="5"/>
         <v>330</v>
       </c>
       <c r="R21" s="10">
-        <f>MOD(P21+270, 360)</f>
+        <f t="shared" si="6"/>
         <v>150</v>
       </c>
       <c r="S21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>510</v>
       </c>
       <c r="T21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>690</v>
       </c>
       <c r="U21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="V21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="W21" t="b">
-        <f t="shared" si="6"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
     </row>
@@ -1494,15 +1684,15 @@
         <v>25</v>
       </c>
       <c r="D22">
-        <f t="shared" ref="D22:F22" si="7">FLOOR(D20,1)</f>
+        <f t="shared" ref="D22:F22" si="14">FLOOR(D20,1)</f>
         <v>11</v>
       </c>
       <c r="E22">
-        <f t="shared" si="7"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="F22" s="10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="G22" s="10">
@@ -1519,42 +1709,42 @@
         <v>90</v>
       </c>
       <c r="M22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="7"/>
         <v>90</v>
       </c>
       <c r="N22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>450</v>
       </c>
       <c r="P22">
         <v>270</v>
       </c>
       <c r="Q22">
-        <f>MOD(P22+90, 360)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="R22">
-        <f>MOD(P22+270, 360)</f>
+        <f t="shared" si="6"/>
         <v>180</v>
       </c>
       <c r="S22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>540</v>
       </c>
       <c r="T22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>720</v>
       </c>
       <c r="U22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="V22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="W22" t="b">
-        <f t="shared" si="6"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
     </row>
@@ -1581,42 +1771,42 @@
         <v>120</v>
       </c>
       <c r="M23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="7"/>
         <v>120</v>
       </c>
       <c r="N23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>480</v>
       </c>
       <c r="P23">
         <v>300</v>
       </c>
       <c r="Q23">
-        <f>MOD(P23+90, 360)</f>
+        <f t="shared" si="5"/>
         <v>30</v>
       </c>
       <c r="R23">
-        <f>MOD(P23+270, 360)</f>
+        <f t="shared" si="6"/>
         <v>210</v>
       </c>
       <c r="S23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>570</v>
       </c>
       <c r="T23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>750</v>
       </c>
       <c r="U23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="V23">
-        <f t="shared" si="5"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="W23" t="b">
-        <f t="shared" si="6"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
     </row>
@@ -1643,42 +1833,42 @@
         <v>150</v>
       </c>
       <c r="M24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="7"/>
         <v>150</v>
       </c>
       <c r="N24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>510</v>
       </c>
       <c r="P24">
         <v>330</v>
       </c>
       <c r="Q24">
-        <f>MOD(P24+90, 360)</f>
+        <f t="shared" si="5"/>
         <v>60</v>
       </c>
       <c r="R24">
-        <f>MOD(P24+270, 360)</f>
+        <f t="shared" si="6"/>
         <v>240</v>
       </c>
       <c r="S24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>600</v>
       </c>
       <c r="T24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>780</v>
       </c>
       <c r="U24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="V24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="W24" t="b">
-        <f t="shared" si="6"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
     </row>
@@ -1687,42 +1877,42 @@
         <v>180</v>
       </c>
       <c r="M25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="7"/>
         <v>180</v>
       </c>
       <c r="N25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>540</v>
       </c>
       <c r="P25">
         <v>360</v>
       </c>
       <c r="Q25">
-        <f>MOD(P25+90, 360)</f>
+        <f t="shared" si="5"/>
         <v>90</v>
       </c>
       <c r="R25">
-        <f>MOD(P25+270, 360)</f>
+        <f t="shared" si="6"/>
         <v>270</v>
       </c>
       <c r="S25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>630</v>
       </c>
       <c r="T25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>810</v>
       </c>
       <c r="U25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="V25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="W25" t="b">
-        <f t="shared" si="6"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
     </row>
@@ -1765,15 +1955,15 @@
         <v>15</v>
       </c>
       <c r="D27" s="1">
-        <f t="shared" ref="D27:F27" si="8">D26/D23</f>
+        <f t="shared" ref="D27:F27" si="15">D26/D23</f>
         <v>0.50750199000000007</v>
       </c>
       <c r="E27" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="15"/>
         <v>4.3750171551724129E-2</v>
       </c>
       <c r="F27" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="15"/>
         <v>4.3772046637499999E-2</v>
       </c>
       <c r="G27" s="1">
@@ -1821,15 +2011,15 @@
         <v>15</v>
       </c>
       <c r="D30" s="1">
-        <f t="shared" ref="D30:F30" si="9">D29/D23</f>
+        <f t="shared" ref="D30:F30" si="16">D29/D23</f>
         <v>4.9378572000000007</v>
       </c>
       <c r="E30" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>0.42567734482758612</v>
       </c>
       <c r="F30" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>0.42589018350000002</v>
       </c>
       <c r="G30" s="1">
@@ -1889,15 +2079,15 @@
         <v>15</v>
       </c>
       <c r="D35" s="1">
-        <f t="shared" ref="D35:F35" si="10">D26*D$33*D$32</f>
+        <f t="shared" ref="D35:F35" si="17">D26*D$33*D$32</f>
         <v>1.3804054128000003</v>
       </c>
       <c r="E35" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="17"/>
         <v>0.11900046662068964</v>
       </c>
       <c r="F35" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="17"/>
         <v>0.119059966854</v>
       </c>
       <c r="G35" s="1">
@@ -1920,15 +2110,15 @@
         <v>15</v>
       </c>
       <c r="D36" s="1">
-        <f t="shared" ref="D36:F36" si="11">D27*D$33*D$32</f>
+        <f t="shared" ref="D36:F36" si="18">D27*D$33*D$32</f>
         <v>0.17255067660000004</v>
       </c>
       <c r="E36" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="18"/>
         <v>1.4875058327586205E-2</v>
       </c>
       <c r="F36" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="18"/>
         <v>1.488249585675E-2</v>
       </c>
       <c r="G36" s="1">
@@ -1956,15 +2146,15 @@
         <v>15</v>
       </c>
       <c r="D38" s="1">
-        <f t="shared" ref="D38:F38" si="12">D29*D$33*D$32</f>
+        <f t="shared" ref="D38:F38" si="19">D29*D$33*D$32</f>
         <v>13.430971584000002</v>
       </c>
       <c r="E38" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="19"/>
         <v>1.1578423779310343</v>
       </c>
       <c r="F38" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="19"/>
         <v>1.1584212991200002</v>
       </c>
       <c r="G38" s="1">
@@ -1984,15 +2174,15 @@
         <v>15</v>
       </c>
       <c r="D39" s="1">
-        <f t="shared" ref="D39:F39" si="13">D30*D$33*D$32</f>
+        <f t="shared" ref="D39:F39" si="20">D30*D$33*D$32</f>
         <v>1.6788714480000002</v>
       </c>
       <c r="E39" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="20"/>
         <v>0.14473029724137929</v>
       </c>
       <c r="F39" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="20"/>
         <v>0.14480266239000003</v>
       </c>
       <c r="G39" s="1">
@@ -2434,12 +2624,13 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="56d601e6-bef3-45c8-b6dc-25c3b07e1d58">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2629,19 +2820,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="56d601e6-bef3-45c8-b6dc-25c3b07e1d58">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5C6F309-A1A2-46F0-A57B-68684D972651}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7469B838-CC0E-428C-B339-A9883501F19C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="56d601e6-bef3-45c8-b6dc-25c3b07e1d58"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2665,11 +2857,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7469B838-CC0E-428C-B339-A9883501F19C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5C6F309-A1A2-46F0-A57B-68684D972651}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="56d601e6-bef3-45c8-b6dc-25c3b07e1d58"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
analysis updates for vector calculation of az and elev
</commit_message>
<xml_diff>
--- a/CCP Laser feasibility study.xlsx
+++ b/CCP Laser feasibility study.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nuitenbr/Desktop/lunarspark/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD807EFE-F0A7-CE4A-8E9D-B07C9EB70685}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE4F3799-F699-2148-8E49-5D7B3DFD46AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="300" yWindow="2760" windowWidth="34720" windowHeight="18880" xr2:uid="{0D0644B8-F9A6-4A61-A91E-2BD3522A7E9F}"/>
+    <workbookView xWindow="1440" yWindow="4500" windowWidth="31040" windowHeight="16040" activeTab="2" xr2:uid="{0D0644B8-F9A6-4A61-A91E-2BD3522A7E9F}"/>
   </bookViews>
   <sheets>
     <sheet name="SE analysis" sheetId="1" r:id="rId1"/>
     <sheet name="fleet cost analysis" sheetId="2" r:id="rId2"/>
+    <sheet name="math" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="102">
   <si>
     <t>baseline</t>
   </si>
@@ -250,16 +251,110 @@
   </si>
   <si>
     <t>lat</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>deg</t>
+  </si>
+  <si>
+    <t>rad</t>
+  </si>
+  <si>
+    <t>cos(theta)</t>
+  </si>
+  <si>
+    <t>sin(theta)</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>cos(phi)</t>
+  </si>
+  <si>
+    <t>sin(phi)</t>
+  </si>
+  <si>
+    <t>-sin(phi)</t>
+  </si>
+  <si>
+    <t>-sin(theta)</t>
+  </si>
+  <si>
+    <t>long</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Z</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>Radius</t>
+  </si>
+  <si>
+    <t>veh</t>
+  </si>
+  <si>
+    <t>sat</t>
+  </si>
+  <si>
+    <t>sat-veh</t>
+  </si>
+  <si>
+    <t>R2R1</t>
+  </si>
+  <si>
+    <t>linear</t>
+  </si>
+  <si>
+    <t>perp</t>
+  </si>
+  <si>
+    <t>phi=90-L</t>
+  </si>
+  <si>
+    <t>theta=long</t>
+  </si>
+  <si>
+    <t>Az (rad)</t>
+  </si>
+  <si>
+    <t>Az (deg)</t>
+  </si>
+  <si>
+    <t>El (rad)</t>
+  </si>
+  <si>
+    <t>El (deg)</t>
+  </si>
+  <si>
+    <t>radius</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="169" formatCode="0.000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -273,8 +368,16 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -299,6 +402,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -312,7 +421,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -330,6 +439,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -646,7 +780,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96B0B46A-223E-4370-BADF-6F68045EC825}">
   <dimension ref="B1:W39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <selection activeCell="V6" sqref="V6"/>
     </sheetView>
   </sheetViews>
@@ -2623,14 +2757,576 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83E790B1-52D8-A842-8268-804FFB128667}">
+  <dimension ref="A2:R25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="2" spans="1:18" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="G2" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="H2" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="I2" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="J2" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="K2" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="L2" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="M2" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="O2" s="21"/>
+      <c r="P2" s="21"/>
+      <c r="Q2" s="21"/>
+      <c r="R2" s="21"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" s="19">
+        <v>90</v>
+      </c>
+      <c r="C3" s="6">
+        <f>B3</f>
+        <v>90</v>
+      </c>
+      <c r="D3" s="15">
+        <f>C3*PI()/180</f>
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="E3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F3" s="16">
+        <f>COS(D3)*COS(D4)*$B5</f>
+        <v>1.0873192537314003E-13</v>
+      </c>
+      <c r="G3" s="16">
+        <f>SIN(D3)*COS(D4)*$B5</f>
+        <v>1775</v>
+      </c>
+      <c r="H3" s="16">
+        <f>SIN(D4)*$B5</f>
+        <v>0</v>
+      </c>
+      <c r="I3" s="16">
+        <f>SQRT(F3*F3+G3*G3+H3*H3)</f>
+        <v>1775</v>
+      </c>
+      <c r="J3" s="15">
+        <f>ATAN((G3/F3))</f>
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="K3" s="16">
+        <f>J3*180/PI()</f>
+        <v>90</v>
+      </c>
+      <c r="L3" s="15">
+        <f>ASIN(H3/I3)</f>
+        <v>0</v>
+      </c>
+      <c r="M3" s="16">
+        <f>L3*180/PI()</f>
+        <v>0</v>
+      </c>
+      <c r="O3" s="14"/>
+      <c r="P3" s="14"/>
+      <c r="Q3" s="18"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4" s="19">
+        <v>0</v>
+      </c>
+      <c r="C4" s="6">
+        <f>B4</f>
+        <v>0</v>
+      </c>
+      <c r="D4" s="15">
+        <f>C4*PI()/180</f>
+        <v>0</v>
+      </c>
+      <c r="E4" t="s">
+        <v>90</v>
+      </c>
+      <c r="F4" s="16">
+        <f>COS(D8)*COS(D9)*$B10</f>
+        <v>-1373</v>
+      </c>
+      <c r="G4" s="16">
+        <f>SIN(D8)*COS(D9)*$B10</f>
+        <v>1.6821288285895353E-13</v>
+      </c>
+      <c r="H4" s="16">
+        <f>SIN(D9)*$B10</f>
+        <v>0</v>
+      </c>
+      <c r="I4" s="16">
+        <f>SQRT(F4*F4+G4*G4+H4*H4)</f>
+        <v>1373</v>
+      </c>
+      <c r="J4" s="15">
+        <f>ATAN((G4/F4))</f>
+        <v>-1.22514845490862E-16</v>
+      </c>
+      <c r="K4" s="16">
+        <f>J4*180/PI()</f>
+        <v>-7.0195835743237771E-15</v>
+      </c>
+      <c r="L4" s="15">
+        <f>ASIN(H4/I4)</f>
+        <v>0</v>
+      </c>
+      <c r="M4" s="16">
+        <f>L4*180/PI()</f>
+        <v>0</v>
+      </c>
+      <c r="Q4" s="18"/>
+      <c r="R4" s="18"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B5" s="19">
+        <f>1373+402</f>
+        <v>1775</v>
+      </c>
+      <c r="E5" t="s">
+        <v>91</v>
+      </c>
+      <c r="F5" s="16">
+        <f>F4-F3</f>
+        <v>-1373</v>
+      </c>
+      <c r="G5" s="16">
+        <f>G4-G3</f>
+        <v>-1774.9999999999998</v>
+      </c>
+      <c r="H5" s="16">
+        <f>H4-H3</f>
+        <v>0</v>
+      </c>
+      <c r="I5" s="16">
+        <f>SQRT(F5*F5+G5*G5+H5*H5)</f>
+        <v>2244.0485734493359</v>
+      </c>
+      <c r="J5" s="15">
+        <f>ATAN((G5/F5))</f>
+        <v>0.91241085511833719</v>
+      </c>
+      <c r="K5" s="16">
+        <f>J5*180/PI()</f>
+        <v>52.27729118020315</v>
+      </c>
+      <c r="L5" s="15">
+        <f>ASIN(H5/I5)</f>
+        <v>0</v>
+      </c>
+      <c r="M5" s="16">
+        <f>L5*180/PI()</f>
+        <v>0</v>
+      </c>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="C6" s="6"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="14"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="6"/>
+    </row>
+    <row r="7" spans="1:18" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="D7" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="E7" s="23"/>
+      <c r="F7" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="G7" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="H7" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="I7" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="J7" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="K7" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="L7" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="M7" s="21" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>81</v>
+      </c>
+      <c r="B8" s="19">
+        <v>180</v>
+      </c>
+      <c r="C8" s="6">
+        <f>B8</f>
+        <v>180</v>
+      </c>
+      <c r="D8" s="15">
+        <f>C8*PI()/180</f>
+        <v>3.1415926535897931</v>
+      </c>
+      <c r="E8" t="s">
+        <v>91</v>
+      </c>
+      <c r="F8" s="16">
+        <f>F5*I18+G5*I19+H5*I20</f>
+        <v>1.0873192537314001E-13</v>
+      </c>
+      <c r="G8" s="16">
+        <f>F5*J18+G5*J19+H5*J20</f>
+        <v>-1373</v>
+      </c>
+      <c r="H8" s="16">
+        <f>F5*K18+G5*K19+H5*K20</f>
+        <v>1.9283836680261679E-13</v>
+      </c>
+      <c r="I8" s="16">
+        <f>SQRT(F8*F8+G8*G8+H8*H8)</f>
+        <v>1373</v>
+      </c>
+      <c r="J8" s="15">
+        <f>ATAN((G8/F8))</f>
+        <v>-1.5707963267948966</v>
+      </c>
+      <c r="K8" s="16">
+        <f>J8*180/PI()</f>
+        <v>-90</v>
+      </c>
+      <c r="L8" s="15">
+        <f>ASIN(F8/I8)</f>
+        <v>7.9192953658514207E-17</v>
+      </c>
+      <c r="M8" s="14">
+        <f>L8*180/PI()</f>
+        <v>4.537422011807976E-15</v>
+      </c>
+      <c r="O8" s="6"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="6"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>70</v>
+      </c>
+      <c r="B9" s="19">
+        <v>0</v>
+      </c>
+      <c r="C9" s="6">
+        <f>B9</f>
+        <v>0</v>
+      </c>
+      <c r="D9" s="15">
+        <f>C9*PI()/180</f>
+        <v>0</v>
+      </c>
+      <c r="N9" s="14"/>
+      <c r="O9" s="14"/>
+      <c r="P9" s="18"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>88</v>
+      </c>
+      <c r="B10" s="19">
+        <v>1373</v>
+      </c>
+      <c r="H10" t="s">
+        <v>93</v>
+      </c>
+      <c r="I10">
+        <f>1775*2-402</f>
+        <v>3148</v>
+      </c>
+      <c r="P10" s="18"/>
+      <c r="Q10" s="18"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="H11" t="s">
+        <v>94</v>
+      </c>
+      <c r="I11" s="3">
+        <f>SQRT(B5*B5+B10*B10)</f>
+        <v>2244.0485734493359</v>
+      </c>
+      <c r="M11" s="18"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="M12" s="18"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="M13" s="18"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="L14" s="14"/>
+      <c r="M14" s="18"/>
+    </row>
+    <row r="17" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="E17" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I17" s="20" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="14">
+        <f>COS(D3)</f>
+        <v>6.1257422745431001E-17</v>
+      </c>
+      <c r="B18" s="14">
+        <f>SIN(D3)</f>
+        <v>1</v>
+      </c>
+      <c r="C18" s="16">
+        <v>0</v>
+      </c>
+      <c r="E18" s="14">
+        <f>COS(PI()/2-D4)</f>
+        <v>6.1257422745431001E-17</v>
+      </c>
+      <c r="F18" s="6">
+        <v>0</v>
+      </c>
+      <c r="G18" s="17">
+        <f>-SIN(PI()/2-D4)</f>
+        <v>-1</v>
+      </c>
+      <c r="I18" s="14">
+        <f>E18*A18+E19*B18+E20*C18</f>
+        <v>3.7524718414124473E-33</v>
+      </c>
+      <c r="J18" s="14">
+        <f>F18*A18+F19*B18+F20*C18</f>
+        <v>1</v>
+      </c>
+      <c r="K18" s="14">
+        <f>G18*A18+G19*B18+G20*C18</f>
+        <v>-6.1257422745431001E-17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="14">
+        <f>-SIN(D3)</f>
+        <v>-1</v>
+      </c>
+      <c r="B19" s="14">
+        <f>COS(D3)</f>
+        <v>6.1257422745431001E-17</v>
+      </c>
+      <c r="C19" s="16">
+        <v>0</v>
+      </c>
+      <c r="E19" s="6">
+        <v>0</v>
+      </c>
+      <c r="F19" s="6">
+        <v>1</v>
+      </c>
+      <c r="G19" s="6">
+        <v>0</v>
+      </c>
+      <c r="I19" s="14">
+        <f>E18*A19+E19*B19+E20*C19</f>
+        <v>-6.1257422745431001E-17</v>
+      </c>
+      <c r="J19" s="14">
+        <f>F18*A19+F19*B19+F20*C19</f>
+        <v>6.1257422745431001E-17</v>
+      </c>
+      <c r="K19" s="14">
+        <f>G18*B19+G19*C19+G20*D19</f>
+        <v>-6.1257422745431001E-17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="6">
+        <v>0</v>
+      </c>
+      <c r="B20" s="6">
+        <v>0</v>
+      </c>
+      <c r="C20" s="16">
+        <v>1</v>
+      </c>
+      <c r="E20" s="14">
+        <f>SIN(PI()/2-D4)</f>
+        <v>1</v>
+      </c>
+      <c r="F20" s="6">
+        <v>0</v>
+      </c>
+      <c r="G20" s="14">
+        <f>COS(PI()/2-D4)</f>
+        <v>6.1257422745431001E-17</v>
+      </c>
+      <c r="I20" s="14">
+        <f>E18*A20+E19*B20+E20*C20</f>
+        <v>1</v>
+      </c>
+      <c r="J20" s="14">
+        <f>F18*A20+F19*B20+F20*C20</f>
+        <v>0</v>
+      </c>
+      <c r="K20" s="14">
+        <f>G18*B20+G19*C20+G20*D20</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="16"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="14"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="14"/>
+      <c r="K21" s="14"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>96</v>
+      </c>
+      <c r="E22" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C23" s="6">
+        <v>0</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="F23" s="6">
+        <v>0</v>
+      </c>
+      <c r="G23" s="13" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C24" s="6">
+        <v>0</v>
+      </c>
+      <c r="E24" s="6">
+        <v>0</v>
+      </c>
+      <c r="F24" s="6">
+        <v>1</v>
+      </c>
+      <c r="G24" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25" s="6">
+        <v>0</v>
+      </c>
+      <c r="B25" s="6">
+        <v>0</v>
+      </c>
+      <c r="C25" s="6">
+        <v>1</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F25" s="6">
+        <v>0</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="56d601e6-bef3-45c8-b6dc-25c3b07e1d58">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2820,20 +3516,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="56d601e6-bef3-45c8-b6dc-25c3b07e1d58">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7469B838-CC0E-428C-B339-A9883501F19C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5C6F309-A1A2-46F0-A57B-68684D972651}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="56d601e6-bef3-45c8-b6dc-25c3b07e1d58"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2857,9 +3552,11 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5C6F309-A1A2-46F0-A57B-68684D972651}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7469B838-CC0E-428C-B339-A9883501F19C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="56d601e6-bef3-45c8-b6dc-25c3b07e1d58"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
added satLat satLong to datastore, need to fix satLong
</commit_message>
<xml_diff>
--- a/CCP Laser feasibility study.xlsx
+++ b/CCP Laser feasibility study.xlsx
@@ -1,37 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nuitenbr/Desktop/lunarspark/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE4F3799-F699-2148-8E49-5D7B3DFD46AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{822A1ACD-08DC-FB47-A930-195AB94840D8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="4500" windowWidth="31040" windowHeight="16040" activeTab="2" xr2:uid="{0D0644B8-F9A6-4A61-A91E-2BD3522A7E9F}"/>
+    <workbookView xWindow="0" yWindow="1960" windowWidth="28800" windowHeight="16040" activeTab="2" xr2:uid="{0D0644B8-F9A6-4A61-A91E-2BD3522A7E9F}"/>
   </bookViews>
   <sheets>
     <sheet name="SE analysis" sheetId="1" r:id="rId1"/>
     <sheet name="fleet cost analysis" sheetId="2" r:id="rId2"/>
     <sheet name="math" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -352,7 +341,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="169" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -436,13 +425,10 @@
     <xf numFmtId="9" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -451,10 +437,10 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -463,7 +449,10 @@
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -479,6 +468,823 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1631427936"/>
+        <c:axId val="1631414496"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1631427936"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1631414496"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1631414496"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1631427936"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>641350</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>260350</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{22B5F3D5-999B-5748-A47B-B09E9850E435}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1720,10 +2526,10 @@
         <f>H18/21*60*H19</f>
         <v>4.0020156925714288</v>
       </c>
-      <c r="I20" s="12" t="s">
+      <c r="I20" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="J20" s="12"/>
+      <c r="J20" s="23"/>
       <c r="L20">
         <v>30</v>
       </c>
@@ -1768,8 +2574,8 @@
       </c>
     </row>
     <row r="21" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="I21" s="12"/>
-      <c r="J21" s="12"/>
+      <c r="I21" s="23"/>
+      <c r="J21" s="23"/>
       <c r="L21">
         <v>60</v>
       </c>
@@ -1837,8 +2643,8 @@
         <f>FLOOR(H20,1)</f>
         <v>4</v>
       </c>
-      <c r="I22" s="12"/>
-      <c r="J22" s="12"/>
+      <c r="I22" s="23"/>
+      <c r="J22" s="23"/>
       <c r="L22">
         <v>90</v>
       </c>
@@ -2759,336 +3565,333 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83E790B1-52D8-A842-8268-804FFB128667}">
-  <dimension ref="A2:R25"/>
+  <dimension ref="A2:Q25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2" spans="1:18" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="20" t="s">
+    <row r="2" spans="1:17" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="F2" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="G2" s="21" t="s">
+      <c r="G2" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="H2" s="21" t="s">
+      <c r="H2" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="I2" s="21" t="s">
+      <c r="I2" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="J2" s="21" t="s">
+      <c r="J2" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="K2" s="21" t="s">
+      <c r="K2" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="L2" s="21" t="s">
+      <c r="L2" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="M2" s="21" t="s">
+      <c r="M2" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="O2" s="21"/>
-      <c r="P2" s="21"/>
-      <c r="Q2" s="21"/>
-      <c r="R2" s="21"/>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="O2" s="20"/>
+      <c r="P2" s="20"/>
+      <c r="Q2" s="20"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>81</v>
       </c>
-      <c r="B3" s="19">
+      <c r="B3" s="18">
         <v>90</v>
       </c>
       <c r="C3" s="6">
         <f>B3</f>
         <v>90</v>
       </c>
-      <c r="D3" s="15">
+      <c r="D3" s="14">
         <f>C3*PI()/180</f>
         <v>1.5707963267948966</v>
       </c>
       <c r="E3" t="s">
         <v>89</v>
       </c>
-      <c r="F3" s="16">
+      <c r="F3" s="15">
         <f>COS(D3)*COS(D4)*$B5</f>
         <v>1.0873192537314003E-13</v>
       </c>
-      <c r="G3" s="16">
+      <c r="G3" s="15">
         <f>SIN(D3)*COS(D4)*$B5</f>
         <v>1775</v>
       </c>
-      <c r="H3" s="16">
+      <c r="H3" s="15">
         <f>SIN(D4)*$B5</f>
         <v>0</v>
       </c>
-      <c r="I3" s="16">
+      <c r="I3" s="15">
         <f>SQRT(F3*F3+G3*G3+H3*H3)</f>
         <v>1775</v>
       </c>
-      <c r="J3" s="15">
+      <c r="J3" s="14">
         <f>ATAN((G3/F3))</f>
         <v>1.5707963267948966</v>
       </c>
-      <c r="K3" s="16">
+      <c r="K3" s="15">
         <f>J3*180/PI()</f>
         <v>90</v>
       </c>
-      <c r="L3" s="15">
+      <c r="L3" s="14">
         <f>ASIN(H3/I3)</f>
         <v>0</v>
       </c>
-      <c r="M3" s="16">
+      <c r="M3" s="15">
         <f>L3*180/PI()</f>
         <v>0</v>
       </c>
-      <c r="O3" s="14"/>
-      <c r="P3" s="14"/>
-      <c r="Q3" s="18"/>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="O3" s="13"/>
+      <c r="P3" s="13"/>
+      <c r="Q3" s="17"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>70</v>
       </c>
-      <c r="B4" s="19">
+      <c r="B4" s="18">
         <v>0</v>
       </c>
       <c r="C4" s="6">
         <f>B4</f>
         <v>0</v>
       </c>
-      <c r="D4" s="15">
+      <c r="D4" s="14">
         <f>C4*PI()/180</f>
         <v>0</v>
       </c>
       <c r="E4" t="s">
         <v>90</v>
       </c>
-      <c r="F4" s="16">
+      <c r="F4" s="15">
         <f>COS(D8)*COS(D9)*$B10</f>
         <v>-1373</v>
       </c>
-      <c r="G4" s="16">
+      <c r="G4" s="15">
         <f>SIN(D8)*COS(D9)*$B10</f>
         <v>1.6821288285895353E-13</v>
       </c>
-      <c r="H4" s="16">
+      <c r="H4" s="15">
         <f>SIN(D9)*$B10</f>
         <v>0</v>
       </c>
-      <c r="I4" s="16">
+      <c r="I4" s="15">
         <f>SQRT(F4*F4+G4*G4+H4*H4)</f>
         <v>1373</v>
       </c>
-      <c r="J4" s="15">
+      <c r="J4" s="14">
         <f>ATAN((G4/F4))</f>
         <v>-1.22514845490862E-16</v>
       </c>
-      <c r="K4" s="16">
+      <c r="K4" s="15">
         <f>J4*180/PI()</f>
         <v>-7.0195835743237771E-15</v>
       </c>
-      <c r="L4" s="15">
+      <c r="L4" s="14">
         <f>ASIN(H4/I4)</f>
         <v>0</v>
       </c>
-      <c r="M4" s="16">
+      <c r="M4" s="15">
         <f>L4*180/PI()</f>
         <v>0</v>
       </c>
-      <c r="Q4" s="18"/>
-      <c r="R4" s="18"/>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="Q4" s="17"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>88</v>
       </c>
-      <c r="B5" s="19">
+      <c r="B5" s="18">
         <f>1373+402</f>
         <v>1775</v>
       </c>
       <c r="E5" t="s">
         <v>91</v>
       </c>
-      <c r="F5" s="16">
+      <c r="F5" s="15">
         <f>F4-F3</f>
         <v>-1373</v>
       </c>
-      <c r="G5" s="16">
+      <c r="G5" s="15">
         <f>G4-G3</f>
         <v>-1774.9999999999998</v>
       </c>
-      <c r="H5" s="16">
+      <c r="H5" s="15">
         <f>H4-H3</f>
         <v>0</v>
       </c>
-      <c r="I5" s="16">
+      <c r="I5" s="15">
         <f>SQRT(F5*F5+G5*G5+H5*H5)</f>
         <v>2244.0485734493359</v>
       </c>
-      <c r="J5" s="15">
+      <c r="J5" s="14">
         <f>ATAN((G5/F5))</f>
         <v>0.91241085511833719</v>
       </c>
-      <c r="K5" s="16">
+      <c r="K5" s="15">
         <f>J5*180/PI()</f>
         <v>52.27729118020315</v>
       </c>
-      <c r="L5" s="15">
+      <c r="L5" s="14">
         <f>ASIN(H5/I5)</f>
         <v>0</v>
       </c>
-      <c r="M5" s="16">
+      <c r="M5" s="15">
         <f>L5*180/PI()</f>
         <v>0</v>
       </c>
       <c r="O5" s="6"/>
       <c r="P5" s="6"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C6" s="6"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
       <c r="I6" s="6"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
       <c r="L6" s="6"/>
-      <c r="M6" s="14"/>
+      <c r="M6" s="13"/>
       <c r="O6" s="6"/>
       <c r="P6" s="6"/>
     </row>
-    <row r="7" spans="1:18" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="20" t="s">
+    <row r="7" spans="1:17" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="D7" s="22" t="s">
+      <c r="D7" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="E7" s="23"/>
-      <c r="F7" s="21" t="s">
+      <c r="E7" s="22"/>
+      <c r="F7" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="G7" s="21" t="s">
+      <c r="G7" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="H7" s="21" t="s">
+      <c r="H7" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="I7" s="21" t="s">
+      <c r="I7" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="J7" s="21" t="s">
+      <c r="J7" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="K7" s="21" t="s">
+      <c r="K7" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="L7" s="21" t="s">
+      <c r="L7" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="M7" s="21" t="s">
+      <c r="M7" s="20" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>81</v>
       </c>
-      <c r="B8" s="19">
+      <c r="B8" s="18">
         <v>180</v>
       </c>
       <c r="C8" s="6">
         <f>B8</f>
         <v>180</v>
       </c>
-      <c r="D8" s="15">
+      <c r="D8" s="14">
         <f>C8*PI()/180</f>
         <v>3.1415926535897931</v>
       </c>
       <c r="E8" t="s">
         <v>91</v>
       </c>
-      <c r="F8" s="16">
+      <c r="F8" s="15">
         <f>F5*I18+G5*I19+H5*I20</f>
         <v>1.0873192537314001E-13</v>
       </c>
-      <c r="G8" s="16">
+      <c r="G8" s="15">
         <f>F5*J18+G5*J19+H5*J20</f>
         <v>-1373</v>
       </c>
-      <c r="H8" s="16">
+      <c r="H8" s="15">
         <f>F5*K18+G5*K19+H5*K20</f>
         <v>1.9283836680261679E-13</v>
       </c>
-      <c r="I8" s="16">
+      <c r="I8" s="15">
         <f>SQRT(F8*F8+G8*G8+H8*H8)</f>
         <v>1373</v>
       </c>
-      <c r="J8" s="15">
+      <c r="J8" s="14">
         <f>ATAN((G8/F8))</f>
         <v>-1.5707963267948966</v>
       </c>
-      <c r="K8" s="16">
+      <c r="K8" s="15">
         <f>J8*180/PI()</f>
         <v>-90</v>
       </c>
-      <c r="L8" s="15">
+      <c r="L8" s="14">
         <f>ASIN(F8/I8)</f>
         <v>7.9192953658514207E-17</v>
       </c>
-      <c r="M8" s="14">
+      <c r="M8" s="13">
         <f>L8*180/PI()</f>
         <v>4.537422011807976E-15</v>
       </c>
       <c r="O8" s="6"/>
       <c r="P8" s="6"/>
       <c r="Q8" s="6"/>
-      <c r="R8" s="6"/>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>70</v>
       </c>
-      <c r="B9" s="19">
+      <c r="B9" s="18">
         <v>0</v>
       </c>
       <c r="C9" s="6">
         <f>B9</f>
         <v>0</v>
       </c>
-      <c r="D9" s="15">
+      <c r="D9" s="14">
         <f>C9*PI()/180</f>
         <v>0</v>
       </c>
-      <c r="N9" s="14"/>
-      <c r="O9" s="14"/>
-      <c r="P9" s="18"/>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="N9" s="13"/>
+      <c r="O9" s="13"/>
+      <c r="P9" s="17"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>88</v>
       </c>
-      <c r="B10" s="19">
+      <c r="B10" s="18">
         <v>1373</v>
       </c>
       <c r="H10" t="s">
@@ -3098,10 +3901,10 @@
         <f>1775*2-402</f>
         <v>3148</v>
       </c>
-      <c r="P10" s="18"/>
-      <c r="Q10" s="18"/>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="P10" s="17"/>
+      <c r="Q10" s="17"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="H11" t="s">
         <v>94</v>
       </c>
@@ -3109,75 +3912,75 @@
         <f>SQRT(B5*B5+B10*B10)</f>
         <v>2244.0485734493359</v>
       </c>
-      <c r="M11" s="18"/>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="M12" s="18"/>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="M13" s="18"/>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="L14" s="14"/>
-      <c r="M14" s="18"/>
-    </row>
-    <row r="17" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="20" t="s">
+      <c r="M11" s="17"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="M12" s="17"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="M13" s="17"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="L14" s="13"/>
+      <c r="M14" s="17"/>
+    </row>
+    <row r="17" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="E17" s="20" t="s">
+      <c r="E17" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="I17" s="20" t="s">
+      <c r="I17" s="19" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A18" s="14">
+      <c r="A18" s="13">
         <f>COS(D3)</f>
         <v>6.1257422745431001E-17</v>
       </c>
-      <c r="B18" s="14">
+      <c r="B18" s="13">
         <f>SIN(D3)</f>
         <v>1</v>
       </c>
-      <c r="C18" s="16">
-        <v>0</v>
-      </c>
-      <c r="E18" s="14">
+      <c r="C18" s="15">
+        <v>0</v>
+      </c>
+      <c r="E18" s="13">
         <f>COS(PI()/2-D4)</f>
         <v>6.1257422745431001E-17</v>
       </c>
       <c r="F18" s="6">
         <v>0</v>
       </c>
-      <c r="G18" s="17">
+      <c r="G18" s="16">
         <f>-SIN(PI()/2-D4)</f>
         <v>-1</v>
       </c>
-      <c r="I18" s="14">
+      <c r="I18" s="13">
         <f>E18*A18+E19*B18+E20*C18</f>
         <v>3.7524718414124473E-33</v>
       </c>
-      <c r="J18" s="14">
+      <c r="J18" s="13">
         <f>F18*A18+F19*B18+F20*C18</f>
         <v>1</v>
       </c>
-      <c r="K18" s="14">
+      <c r="K18" s="13">
         <f>G18*A18+G19*B18+G20*C18</f>
         <v>-6.1257422745431001E-17</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A19" s="14">
+      <c r="A19" s="13">
         <f>-SIN(D3)</f>
         <v>-1</v>
       </c>
-      <c r="B19" s="14">
+      <c r="B19" s="13">
         <f>COS(D3)</f>
         <v>6.1257422745431001E-17</v>
       </c>
-      <c r="C19" s="16">
+      <c r="C19" s="15">
         <v>0</v>
       </c>
       <c r="E19" s="6">
@@ -3189,15 +3992,15 @@
       <c r="G19" s="6">
         <v>0</v>
       </c>
-      <c r="I19" s="14">
+      <c r="I19" s="13">
         <f>E18*A19+E19*B19+E20*C19</f>
         <v>-6.1257422745431001E-17</v>
       </c>
-      <c r="J19" s="14">
+      <c r="J19" s="13">
         <f>F18*A19+F19*B19+F20*C19</f>
         <v>6.1257422745431001E-17</v>
       </c>
-      <c r="K19" s="14">
+      <c r="K19" s="13">
         <f>G18*B19+G19*C19+G20*D19</f>
         <v>-6.1257422745431001E-17</v>
       </c>
@@ -3209,29 +4012,29 @@
       <c r="B20" s="6">
         <v>0</v>
       </c>
-      <c r="C20" s="16">
+      <c r="C20" s="15">
         <v>1</v>
       </c>
-      <c r="E20" s="14">
+      <c r="E20" s="13">
         <f>SIN(PI()/2-D4)</f>
         <v>1</v>
       </c>
       <c r="F20" s="6">
         <v>0</v>
       </c>
-      <c r="G20" s="14">
+      <c r="G20" s="13">
         <f>COS(PI()/2-D4)</f>
         <v>6.1257422745431001E-17</v>
       </c>
-      <c r="I20" s="14">
+      <c r="I20" s="13">
         <f>E18*A20+E19*B20+E20*C20</f>
         <v>1</v>
       </c>
-      <c r="J20" s="14">
+      <c r="J20" s="13">
         <f>F18*A20+F19*B20+F20*C20</f>
         <v>0</v>
       </c>
-      <c r="K20" s="14">
+      <c r="K20" s="13">
         <f>G18*B20+G19*C20+G20*D20</f>
         <v>0</v>
       </c>
@@ -3239,13 +4042,13 @@
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
-      <c r="C21" s="16"/>
-      <c r="E21" s="14"/>
+      <c r="C21" s="15"/>
+      <c r="E21" s="13"/>
       <c r="F21" s="6"/>
-      <c r="G21" s="14"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="14"/>
-      <c r="K21" s="14"/>
+      <c r="G21" s="13"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="13"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
@@ -3271,12 +4074,12 @@
       <c r="F23" s="6">
         <v>0</v>
       </c>
-      <c r="G23" s="13" t="s">
+      <c r="G23" s="12" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A24" s="13" t="s">
+      <c r="A24" s="12" t="s">
         <v>80</v>
       </c>
       <c r="B24" s="6" t="s">
@@ -3317,19 +4120,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100870398E7EAE9954ABE6BFB497661637E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3786cb5e95af3a90c677764e8014d423">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="56d601e6-bef3-45c8-b6dc-25c3b07e1d58" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="adb27d47ef9772e2cb84c18b7530cab2" ns2:_="">
     <xsd:import namespace="56d601e6-bef3-45c8-b6dc-25c3b07e1d58"/>
@@ -3515,6 +4310,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -3526,14 +4330,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5C6F309-A1A2-46F0-A57B-68684D972651}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD5649D0-F6D4-456F-915F-B334A3145553}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3551,6 +4347,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5C6F309-A1A2-46F0-A57B-68684D972651}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7469B838-CC0E-428C-B339-A9883501F19C}">
   <ds:schemaRefs>

</xml_diff>